<commit_message>
Updated and added json
</commit_message>
<xml_diff>
--- a/covid_19_data_switzerland.xlsx
+++ b/covid_19_data_switzerland.xlsx
@@ -2464,7 +2464,9 @@
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr"/>
+      <c r="C34" t="n">
+        <v>13</v>
+      </c>
       <c r="D34" t="n">
         <v>45</v>
       </c>
@@ -2530,7 +2532,7 @@
         <v>1720</v>
       </c>
       <c r="AB34" t="n">
-        <v>14123</v>
+        <v>14124</v>
       </c>
     </row>
     <row r="35">
@@ -2548,7 +2550,9 @@
         <v>798</v>
       </c>
       <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
+      <c r="G35" t="n">
+        <v>609</v>
+      </c>
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
@@ -2562,7 +2566,9 @@
         <v>365</v>
       </c>
       <c r="R35" t="inlineStr"/>
-      <c r="S35" t="inlineStr"/>
+      <c r="S35" t="n">
+        <v>190</v>
+      </c>
       <c r="T35" t="n">
         <v>128</v>
       </c>
@@ -2574,7 +2580,7 @@
       <c r="Z35" t="inlineStr"/>
       <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="n">
-        <v>14189</v>
+        <v>14243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated and added summary.json
</commit_message>
<xml_diff>
--- a/covid_19_data_switzerland.xlsx
+++ b/covid_19_data_switzerland.xlsx
@@ -2553,7 +2553,9 @@
       <c r="G35" t="n">
         <v>609</v>
       </c>
-      <c r="H35" t="inlineStr"/>
+      <c r="H35" t="n">
+        <v>442</v>
+      </c>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
@@ -2582,7 +2584,7 @@
       <c r="Z35" t="inlineStr"/>
       <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="n">
-        <v>14246</v>
+        <v>14267</v>
       </c>
     </row>
   </sheetData>
@@ -4366,7 +4368,9 @@
       </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
+      <c r="H35" t="n">
+        <v>16</v>
+      </c>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
@@ -4391,7 +4395,7 @@
       <c r="Z35" t="inlineStr"/>
       <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="n">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -6101,7 +6105,9 @@
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
+      <c r="H35" t="n">
+        <v>76</v>
+      </c>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
@@ -6122,7 +6128,7 @@
       <c r="Z35" t="inlineStr"/>
       <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="n">
-        <v>1681</v>
+        <v>1690</v>
       </c>
     </row>
   </sheetData>

</xml_diff>